<commit_message>
uploaded results of llama 2 chunk size benchmarks
</commit_message>
<xml_diff>
--- a/perso/Jules/table_resultats.xlsx
+++ b/perso/Jules/table_resultats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jules\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECFEB430-8132-4596-BB7A-C4BB6B443CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69921724-79A7-4CD2-AFD7-39E5C1CF1593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8565" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{475726F6-9D7E-4144-B407-D3E8354D6C2B}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="218">
   <si>
     <t>intermediate_2/1_3.txt</t>
   </si>
@@ -571,9 +571,6 @@
     <t>falcon-7b-inst</t>
   </si>
   <si>
-    <t>0SL</t>
-  </si>
-  <si>
     <t>ROUGE-1</t>
   </si>
   <si>
@@ -607,12 +604,6 @@
     <t>2SL 1000T</t>
   </si>
   <si>
-    <t>MODEL</t>
-  </si>
-  <si>
-    <t>CHUNK SIZE</t>
-  </si>
-  <si>
     <t>2SL 4bit</t>
   </si>
   <si>
@@ -637,30 +628,18 @@
     <t>15m</t>
   </si>
   <si>
-    <t>PIPELINE (&lt;6k characters)</t>
-  </si>
-  <si>
     <t>Disfluencies</t>
   </si>
   <si>
     <t>20m</t>
   </si>
   <si>
-    <t>Hallucinations (10 samples)</t>
-  </si>
-  <si>
     <t>Hallucinations</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
     <t>Length (tokens)</t>
   </si>
   <si>
-    <t>Ratio (H/S)</t>
-  </si>
-  <si>
     <t>Sample</t>
   </si>
   <si>
@@ -676,14 +655,65 @@
     <t>&lt;5000T</t>
   </si>
   <si>
-    <t>Ratio (H/kT)</t>
+    <t>SUMM-RE</t>
+  </si>
+  <si>
+    <t>0SL 1500T</t>
+  </si>
+  <si>
+    <t>0SL 2000T</t>
+  </si>
+  <si>
+    <t>0SL 3500T</t>
+  </si>
+  <si>
+    <t>0SL 3000T</t>
+  </si>
+  <si>
+    <t>CHUNK SIZE LLAMA</t>
+  </si>
+  <si>
+    <t>CHUNK SIZE XGEN</t>
+  </si>
+  <si>
+    <t>XGEN CHUNK SIZE HALLUCINATIONS</t>
+  </si>
+  <si>
+    <t>0SL 2500T</t>
+  </si>
+  <si>
+    <t>llama-2-7b-chat-hf</t>
+  </si>
+  <si>
+    <t>1SL 3000T</t>
+  </si>
+  <si>
+    <t>MODEL + CHUNK</t>
+  </si>
+  <si>
+    <t>PIPELINE (&lt;6kc)</t>
+  </si>
+  <si>
+    <t>MODEL (0SL &lt;6kc)</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>0SL 1600T</t>
+  </si>
+  <si>
+    <t>Ratio (H/C)</t>
+  </si>
+  <si>
+    <t>Ratio (H/L)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -728,15 +758,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -777,13 +800,8 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1003,15 +1021,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1046,33 +1074,26 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1087,12 +1108,34 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="3" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="4">
     <cellStyle name="20 % - Accent1" xfId="2" builtinId="30"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
-    <cellStyle name="Insatisfaisant" xfId="4" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Satisfaisant" xfId="3" builtinId="26"/>
   </cellStyles>
@@ -1123,6 +1166,66 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>XGen Optimal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> Chunk Sizing</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
@@ -1856,7 +1959,838 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t>LLaMA</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> 2</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR"/>
+              <a:t> Optimal</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="fr-FR" baseline="0"/>
+              <a:t> Chunk Sizing</a:t>
+            </a:r>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chunking!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROUGE-1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Chunking!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0SL 1500T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0SL 2000T</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0SL 2500T</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0SL 3000T</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0SL 3500T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chunking!$D$17:$D$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.243778036353753</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.280795273814541</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30059483315205798</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.32226630914329901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33834132317935101</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5D38-401B-BBAA-02E7F88DDCDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chunking!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROUGE-2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Chunking!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0SL 1500T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0SL 2000T</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0SL 2500T</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0SL 3000T</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0SL 3500T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chunking!$E$17:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>7.4697752541906998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.5582870561372495E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.1788545837451695E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.8757992060049806E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3856469421591598E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-5D38-401B-BBAA-02E7F88DDCDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chunking!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>ROUGE-L</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Chunking!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0SL 1500T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0SL 2000T</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0SL 2500T</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0SL 3000T</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0SL 3500T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chunking!$F$17:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.14683269895611401</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16494646581060199</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.17083391416511601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.18068439336637701</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.190951083508627</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-5D38-401B-BBAA-02E7F88DDCDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chunking!$G$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BERT-Score</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:strRef>
+              <c:f>Chunking!$C$17:$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0SL 1500T</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0SL 2000T</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0SL 2500T</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0SL 3000T</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0SL 3500T</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chunking!$G$17:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.20598052106797601</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.209855249896645</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.22305893748998601</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.217093224078416</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.23476739414036199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-5D38-401B-BBAA-02E7F88DDCDE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="462542496"/>
+        <c:axId val="462539976"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="462542496"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Maximum</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="fr-FR" baseline="0"/>
+                  <a:t> Chunk Size (ktokens)</a:t>
+                </a:r>
+                <a:endParaRPr lang="fr-FR"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="462539976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="462539976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="0.37000000000000005"/>
+          <c:min val="5.000000000000001E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="fr-FR"/>
+                  <a:t>Scores</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="fr-FR"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="462542496"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -2412,20 +3346,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>425450</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2445,6 +3895,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>282575</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Graphique 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6B3E79F3-4D01-47A6-9A82-2E95DB0AE3A8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2764,26 +4252,26 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="28"/>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="L1" s="39" t="s">
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="L1" s="37" t="s">
         <v>127</v>
       </c>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
+      <c r="M1" s="37"/>
+      <c r="N1" s="37"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="27" t="s">
@@ -3005,112 +4493,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5AFC44-E724-4E03-A6C5-1EB9B2C767D1}">
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:R38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.7265625" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="19" max="19" width="10.90625" style="38"/>
+    <col min="2" max="2" width="16.90625" customWidth="1"/>
+    <col min="18" max="18" width="10.90625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A1" s="29"/>
-      <c r="B1" s="41" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B1" s="38" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="38" t="s">
         <v>169</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41" t="s">
-        <v>187</v>
-      </c>
-      <c r="I1" s="44" t="s">
-        <v>197</v>
-      </c>
-      <c r="J1" s="42" t="s">
-        <v>188</v>
-      </c>
-      <c r="K1" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="L1" s="34"/>
-      <c r="S1" s="41" t="s">
-        <v>202</v>
-      </c>
-      <c r="T1" s="39" t="s">
-        <v>198</v>
-      </c>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39" t="s">
-        <v>204</v>
-      </c>
-      <c r="W1" s="39"/>
-      <c r="X1" s="45" t="s">
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" s="40" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="K1" s="38" t="s">
         <v>200</v>
       </c>
-      <c r="Y1" s="46"/>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="29"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="35" t="s">
-        <v>173</v>
-      </c>
-      <c r="E2" s="36" t="s">
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G2" s="36" t="s">
+      <c r="G2" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="43"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="34"/>
-      <c r="S2" s="41"/>
-      <c r="T2" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="U2" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="V2" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="W2" s="28" t="s">
-        <v>206</v>
-      </c>
-      <c r="X2" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="Y2" s="28" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A3" s="40" t="s">
-        <v>194</v>
+      <c r="H2" s="38"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="L2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="M2" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="P2" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q2" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="R2" s="35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="39" t="s">
+        <v>212</v>
       </c>
       <c r="B3" s="29" t="s">
         <v>168</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D3" s="29">
         <v>0.209397095097723</v>
@@ -3124,33 +4607,13 @@
       <c r="G3" s="29">
         <v>0.17726770726342958</v>
       </c>
-      <c r="H3" s="29">
+      <c r="H3" s="54">
         <v>30</v>
       </c>
-      <c r="S3" s="28">
-        <v>10</v>
-      </c>
-      <c r="T3" s="29">
-        <v>1</v>
-      </c>
-      <c r="U3" s="29">
-        <v>0</v>
-      </c>
-      <c r="V3" s="29">
-        <v>10</v>
-      </c>
-      <c r="W3" s="29">
-        <v>2</v>
-      </c>
-      <c r="X3" s="29">
-        <v>1249</v>
-      </c>
-      <c r="Y3" s="29">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A4" s="40"/>
+      <c r="R3"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A4" s="39"/>
       <c r="B4" s="29" t="s">
         <v>168</v>
       </c>
@@ -3169,38 +4632,16 @@
       <c r="G4" s="29">
         <v>0.207062956690788</v>
       </c>
-      <c r="H4" s="29">
-        <v>30</v>
-      </c>
-      <c r="S4" s="28">
-        <v>11</v>
-      </c>
-      <c r="T4" s="29">
-        <v>5</v>
-      </c>
-      <c r="U4" s="29">
-        <v>1</v>
-      </c>
-      <c r="V4" s="29">
-        <v>11</v>
-      </c>
-      <c r="W4" s="29">
-        <v>3</v>
-      </c>
-      <c r="X4" s="29">
-        <v>1472</v>
-      </c>
-      <c r="Y4" s="29">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
+      <c r="H4" s="55"/>
+      <c r="R4"/>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A5" s="39"/>
       <c r="B5" s="29" t="s">
         <v>168</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="29">
         <v>0.29841649238096202</v>
@@ -3214,38 +4655,16 @@
       <c r="G5" s="29">
         <v>0.22586498012145301</v>
       </c>
-      <c r="H5" s="29">
-        <v>30</v>
-      </c>
-      <c r="S5" s="28">
-        <v>12</v>
-      </c>
-      <c r="T5" s="29">
-        <v>12</v>
-      </c>
-      <c r="U5" s="29">
-        <v>2</v>
-      </c>
-      <c r="V5" s="29">
-        <v>12</v>
-      </c>
-      <c r="W5" s="29">
-        <v>3</v>
-      </c>
-      <c r="X5" s="29">
-        <v>1355</v>
-      </c>
-      <c r="Y5" s="29">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A6" s="40"/>
+      <c r="H5" s="55"/>
+      <c r="R5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A6" s="39"/>
       <c r="B6" s="29" t="s">
         <v>168</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="32">
         <v>0.31115736810670003</v>
@@ -3259,40 +4678,18 @@
       <c r="G6" s="32">
         <v>0.23438942184050801</v>
       </c>
-      <c r="H6" s="29">
-        <v>30</v>
-      </c>
-      <c r="S6" s="28">
-        <v>13</v>
-      </c>
-      <c r="T6" s="29">
-        <v>0</v>
-      </c>
-      <c r="U6" s="29">
-        <v>0</v>
-      </c>
-      <c r="V6" s="29">
-        <v>5</v>
-      </c>
-      <c r="W6" s="29">
-        <v>1</v>
-      </c>
-      <c r="X6" s="29">
-        <v>559</v>
-      </c>
-      <c r="Y6" s="29">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A7" s="40" t="s">
-        <v>184</v>
+      <c r="H6" s="56"/>
+      <c r="R6"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A7" s="39" t="s">
+        <v>213</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>168</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="D7" s="29">
         <v>0.26587951816970701</v>
@@ -3309,36 +4706,14 @@
       <c r="H7" s="29">
         <v>30</v>
       </c>
-      <c r="I7" s="33"/>
-      <c r="S7" s="28">
-        <v>14</v>
-      </c>
-      <c r="T7" s="29">
-        <v>4</v>
-      </c>
-      <c r="U7" s="29">
-        <v>1</v>
-      </c>
-      <c r="V7" s="29">
-        <v>7</v>
-      </c>
-      <c r="W7" s="29">
-        <v>2</v>
-      </c>
-      <c r="X7" s="29">
-        <v>809</v>
-      </c>
-      <c r="Y7" s="29">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A8" s="40"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A8" s="39"/>
       <c r="B8" s="29" t="s">
         <v>171</v>
       </c>
       <c r="C8" s="29" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="D8" s="29">
         <v>0.256643614056007</v>
@@ -3355,324 +4730,690 @@
       <c r="H8" s="29">
         <v>12</v>
       </c>
-      <c r="I8" s="33"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A9" s="40"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A9" s="39"/>
       <c r="B9" s="29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>172</v>
+        <v>214</v>
       </c>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="29"/>
       <c r="G9" s="29"/>
       <c r="H9" s="29"/>
-      <c r="I9" s="33"/>
-      <c r="S9" s="28" t="s">
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A10" s="39"/>
+      <c r="B10" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="D10" s="29">
+        <v>0.24629682378621801</v>
+      </c>
+      <c r="E10" s="29">
+        <v>7.60645037007735E-2</v>
+      </c>
+      <c r="F10" s="29">
+        <v>0.14876185272931799</v>
+      </c>
+      <c r="G10" s="29">
+        <v>0.19811991304159099</v>
+      </c>
+      <c r="H10" s="29">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A11" s="39" t="s">
+        <v>206</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="D11" s="29">
+        <v>0.20507990656150499</v>
+      </c>
+      <c r="E11" s="29">
+        <v>6.69138054664003E-2</v>
+      </c>
+      <c r="F11" s="29">
+        <v>0.12402657580828901</v>
+      </c>
+      <c r="G11" s="29">
+        <v>0.19532383158802899</v>
+      </c>
+      <c r="H11" s="54">
+        <v>20</v>
+      </c>
+      <c r="I11" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="J11" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A12" s="39"/>
+      <c r="B12" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="29" t="s">
+        <v>177</v>
+      </c>
+      <c r="D12" s="29">
+        <v>0.25972124903941601</v>
+      </c>
+      <c r="E12" s="29">
+        <v>7.3515387646194294E-2</v>
+      </c>
+      <c r="F12" s="29">
+        <v>0.152574999376515</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0.19273205921053799</v>
+      </c>
+      <c r="H12" s="55"/>
+      <c r="I12" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="J12" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A13" s="39"/>
+      <c r="B13" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="D13" s="29">
+        <v>0.31310274540431099</v>
+      </c>
+      <c r="E13" s="29">
+        <v>8.5520439669621501E-2</v>
+      </c>
+      <c r="F13" s="29">
+        <v>0.185344783555562</v>
+      </c>
+      <c r="G13" s="29">
+        <v>0.185344783555562</v>
+      </c>
+      <c r="H13" s="55"/>
+      <c r="I13" s="29" t="s">
+        <v>190</v>
+      </c>
+      <c r="J13" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A14" s="39"/>
+      <c r="B14" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>179</v>
+      </c>
+      <c r="D14" s="32">
+        <v>0.34665637730130699</v>
+      </c>
+      <c r="E14" s="32">
+        <v>8.6193399759123407E-2</v>
+      </c>
+      <c r="F14" s="32">
+        <v>0.19448828347796701</v>
+      </c>
+      <c r="G14" s="29">
+        <v>0.22589851021766599</v>
+      </c>
+      <c r="H14" s="55"/>
+      <c r="I14" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="J14" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A15" s="39"/>
+      <c r="B15" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="D15" s="29">
+        <v>0.33222808352364203</v>
+      </c>
+      <c r="E15" s="29">
+        <v>8.3754834143228804E-2</v>
+      </c>
+      <c r="F15" s="29">
+        <v>0.19432044552351499</v>
+      </c>
+      <c r="G15" s="32">
+        <v>0.234600452147424</v>
+      </c>
+      <c r="H15" s="55"/>
+      <c r="I15" s="29" t="s">
+        <v>189</v>
+      </c>
+      <c r="J15" s="29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A16" s="39"/>
+      <c r="B16" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="29" t="s">
+        <v>181</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0.32203169576661</v>
+      </c>
+      <c r="E16" s="29">
+        <v>7.0582749966208697E-2</v>
+      </c>
+      <c r="F16" s="29">
+        <v>0.18391282196315101</v>
+      </c>
+      <c r="G16" s="29">
+        <v>0.20042349733412201</v>
+      </c>
+      <c r="H16" s="56"/>
+      <c r="I16" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="J16" s="29">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A17" s="39" t="s">
+        <v>205</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>201</v>
+      </c>
+      <c r="D17" s="47">
+        <v>0.243778036353753</v>
+      </c>
+      <c r="E17" s="47">
+        <v>7.4697752541906998E-2</v>
+      </c>
+      <c r="F17" s="47">
+        <v>0.14683269895611401</v>
+      </c>
+      <c r="G17" s="47">
+        <v>0.20598052106797601</v>
+      </c>
+      <c r="H17" s="51">
+        <v>20</v>
+      </c>
+      <c r="K17" s="46"/>
+      <c r="L17" s="46"/>
+      <c r="M17" s="46"/>
+      <c r="N17" s="46"/>
+      <c r="O17" s="46"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A18" s="39"/>
+      <c r="B18" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>202</v>
+      </c>
+      <c r="D18" s="47">
+        <v>0.280795273814541</v>
+      </c>
+      <c r="E18" s="47">
+        <v>8.5582870561372495E-2</v>
+      </c>
+      <c r="F18" s="47">
+        <v>0.16494646581060199</v>
+      </c>
+      <c r="G18" s="47">
+        <v>0.209855249896645</v>
+      </c>
+      <c r="H18" s="52"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
+      <c r="N18" s="46"/>
+      <c r="O18" s="46"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A19" s="39"/>
+      <c r="B19" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="D19" s="47">
+        <v>0.30059483315205798</v>
+      </c>
+      <c r="E19" s="47">
+        <v>8.1788545837451695E-2</v>
+      </c>
+      <c r="F19" s="47">
+        <v>0.17083391416511601</v>
+      </c>
+      <c r="G19" s="47">
+        <v>0.22305893748998601</v>
+      </c>
+      <c r="H19" s="52"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="46"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A20" s="39"/>
+      <c r="B20" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="D20" s="47">
+        <v>0.32226630914329901</v>
+      </c>
+      <c r="E20" s="49">
+        <v>8.8757992060049806E-2</v>
+      </c>
+      <c r="F20" s="47">
+        <v>0.18068439336637701</v>
+      </c>
+      <c r="G20" s="47">
+        <v>0.217093224078416</v>
+      </c>
+      <c r="H20" s="52"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
+      <c r="M20" s="46"/>
+      <c r="N20" s="46"/>
+      <c r="O20" s="46"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A21" s="39"/>
+      <c r="B21" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="29" t="s">
         <v>203</v>
       </c>
-      <c r="T9" s="29">
-        <f>SUM(T3:T7)</f>
+      <c r="D21" s="49">
+        <v>0.33834132317935101</v>
+      </c>
+      <c r="E21" s="47">
+        <v>8.3856469421591598E-2</v>
+      </c>
+      <c r="F21" s="49">
+        <v>0.190951083508627</v>
+      </c>
+      <c r="G21" s="49">
+        <v>0.23476739414036199</v>
+      </c>
+      <c r="H21" s="53"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A22" s="39" t="s">
+        <v>211</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="C22" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
+      <c r="M22" s="29"/>
+      <c r="N22" s="29"/>
+      <c r="O22" s="29"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="29"/>
+      <c r="R22" s="29"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A23" s="39"/>
+      <c r="B23" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="29"/>
+      <c r="N23" s="29"/>
+      <c r="O23" s="29"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A24" s="39"/>
+      <c r="B24" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="29" t="s">
+        <v>203</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
+      <c r="M24" s="29"/>
+      <c r="N24" s="29"/>
+      <c r="O24" s="29"/>
+      <c r="P24" s="29"/>
+      <c r="Q24" s="29"/>
+      <c r="R24" s="29"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A25" s="39"/>
+      <c r="B25" s="29" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
+      <c r="M25" s="29"/>
+      <c r="N25" s="29"/>
+      <c r="O25" s="29"/>
+      <c r="P25" s="29"/>
+      <c r="Q25" s="29"/>
+      <c r="R25" s="29"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="C26" s="50"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A27" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B27" s="37"/>
+      <c r="C27" s="37"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="37"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A28" s="38" t="s">
+        <v>195</v>
+      </c>
+      <c r="B28" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="37"/>
+      <c r="F28" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="G28" s="43"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A29" s="38"/>
+      <c r="B29" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A30" s="28">
+        <v>10</v>
+      </c>
+      <c r="B30" s="29">
+        <v>1</v>
+      </c>
+      <c r="C30" s="29">
+        <v>0</v>
+      </c>
+      <c r="D30" s="29">
+        <v>10</v>
+      </c>
+      <c r="E30" s="29">
+        <v>2</v>
+      </c>
+      <c r="F30" s="29">
+        <v>1249</v>
+      </c>
+      <c r="G30" s="29">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A31" s="28">
+        <v>11</v>
+      </c>
+      <c r="B31" s="29">
+        <v>5</v>
+      </c>
+      <c r="C31" s="29">
+        <v>1</v>
+      </c>
+      <c r="D31" s="29">
+        <v>11</v>
+      </c>
+      <c r="E31" s="29">
+        <v>3</v>
+      </c>
+      <c r="F31" s="29">
+        <v>1472</v>
+      </c>
+      <c r="G31" s="29">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A32" s="28">
+        <v>12</v>
+      </c>
+      <c r="B32" s="29">
+        <v>12</v>
+      </c>
+      <c r="C32" s="29">
+        <v>2</v>
+      </c>
+      <c r="D32" s="29">
+        <v>12</v>
+      </c>
+      <c r="E32" s="29">
+        <v>3</v>
+      </c>
+      <c r="F32" s="29">
+        <v>1355</v>
+      </c>
+      <c r="G32" s="29">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="28">
+        <v>13</v>
+      </c>
+      <c r="B33" s="29">
+        <v>0</v>
+      </c>
+      <c r="C33" s="29">
+        <v>0</v>
+      </c>
+      <c r="D33" s="29">
+        <v>5</v>
+      </c>
+      <c r="E33" s="29">
+        <v>1</v>
+      </c>
+      <c r="F33" s="29">
+        <v>559</v>
+      </c>
+      <c r="G33" s="29">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="28">
+        <v>14</v>
+      </c>
+      <c r="B34" s="29">
+        <v>4</v>
+      </c>
+      <c r="C34" s="29">
+        <v>1</v>
+      </c>
+      <c r="D34" s="29">
+        <v>7</v>
+      </c>
+      <c r="E34" s="29">
+        <v>2</v>
+      </c>
+      <c r="F34" s="29">
+        <v>809</v>
+      </c>
+      <c r="G34" s="29">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A35" s="36"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A36" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36" s="29">
+        <f>SUM(B30:B34)</f>
         <v>22</v>
       </c>
-      <c r="U9" s="29">
-        <f t="shared" ref="U9:Y9" si="0">SUM(U3:U7)</f>
+      <c r="C36" s="29">
+        <f t="shared" ref="C36:G36" si="0">SUM(C30:C34)</f>
         <v>4</v>
       </c>
-      <c r="V9" s="29">
+      <c r="D36" s="29">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="W9" s="29">
+      <c r="E36" s="29">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="X9" s="29">
+      <c r="F36" s="29">
         <f t="shared" si="0"/>
         <v>5444</v>
       </c>
-      <c r="Y9" s="29">
+      <c r="G36" s="29">
         <f t="shared" si="0"/>
         <v>1291</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A10" s="40"/>
-      <c r="B10" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="C10" s="29" t="s">
-        <v>172</v>
-      </c>
-      <c r="D10" s="29">
-        <v>0.24629682378621801</v>
-      </c>
-      <c r="E10" s="29">
-        <v>7.60645037007735E-2</v>
-      </c>
-      <c r="F10" s="29">
-        <v>0.14876185272931799</v>
-      </c>
-      <c r="G10" s="29">
-        <v>0.19811991304159099</v>
-      </c>
-      <c r="H10" s="29">
-        <v>30</v>
-      </c>
-      <c r="I10" s="33"/>
-      <c r="S10" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="T10" s="29">
-        <f>AVERAGE(T3:T7)</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="U10" s="29">
-        <f>AVERAGE(U3:U7)</f>
-        <v>0.8</v>
-      </c>
-      <c r="V10" s="29">
-        <f>AVERAGE(V3:V7)</f>
-        <v>9</v>
-      </c>
-      <c r="W10" s="29">
-        <f>AVERAGE(W3:W7)</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="X10" s="29">
-        <f>AVERAGE(X3:X7)</f>
-        <v>1088.8</v>
-      </c>
-      <c r="Y10" s="29">
-        <f>AVERAGE(Y3:Y7)</f>
-        <v>258.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A11" s="40" t="s">
-        <v>185</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C11" s="29" t="s">
-        <v>183</v>
-      </c>
-      <c r="D11" s="29">
-        <v>0.20507990656150499</v>
-      </c>
-      <c r="E11" s="29">
-        <v>6.69138054664003E-2</v>
-      </c>
-      <c r="F11" s="29">
-        <v>0.12402657580828901</v>
-      </c>
-      <c r="G11" s="29">
-        <v>0.19532383158802899</v>
-      </c>
-      <c r="H11" s="29">
-        <v>20</v>
-      </c>
-      <c r="I11" s="29"/>
-      <c r="J11" s="29" t="s">
-        <v>189</v>
-      </c>
-      <c r="K11" s="29">
-        <v>0</v>
-      </c>
-      <c r="S11" s="28" t="s">
-        <v>201</v>
-      </c>
-      <c r="T11" s="49">
-        <f>T10/V10</f>
-        <v>0.48888888888888893</v>
-      </c>
-      <c r="U11" s="29">
-        <f>U10/W10</f>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A37" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="B37" s="29">
+        <f>B36/D36</f>
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="C37" s="29">
+        <f>C36/E36</f>
         <v>0.36363636363636365</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A12" s="40"/>
-      <c r="B12" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C12" s="29" t="s">
-        <v>178</v>
-      </c>
-      <c r="D12" s="29">
-        <v>0.25972124903941601</v>
-      </c>
-      <c r="E12" s="29">
-        <v>7.3515387646194294E-2</v>
-      </c>
-      <c r="F12" s="29">
-        <v>0.152574999376515</v>
-      </c>
-      <c r="G12" s="29">
-        <v>0.19273205921053799</v>
-      </c>
-      <c r="H12" s="29">
-        <v>20</v>
-      </c>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29" t="s">
-        <v>190</v>
-      </c>
-      <c r="K12" s="29">
-        <v>1</v>
-      </c>
-      <c r="S12" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="T12" s="49">
-        <f>T10/X10*1000</f>
-        <v>4.0411462160176352</v>
-      </c>
-      <c r="U12" s="29">
-        <f>U10/Y10*1000</f>
-        <v>3.0983733539891558</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A13" s="40"/>
-      <c r="B13" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>179</v>
-      </c>
-      <c r="D13" s="29">
-        <v>0.31310274540431099</v>
-      </c>
-      <c r="E13" s="29">
-        <v>8.5520439669621501E-2</v>
-      </c>
-      <c r="F13" s="29">
-        <v>0.185344783555562</v>
-      </c>
-      <c r="G13" s="29">
-        <v>0.185344783555562</v>
-      </c>
-      <c r="H13" s="29">
-        <v>20</v>
-      </c>
-      <c r="I13" s="29"/>
-      <c r="J13" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="K13" s="29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A14" s="40"/>
-      <c r="B14" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>180</v>
-      </c>
-      <c r="D14" s="32">
-        <v>0.34665637730130699</v>
-      </c>
-      <c r="E14" s="32">
-        <v>8.6193399759123407E-2</v>
-      </c>
-      <c r="F14" s="32">
-        <v>0.19448828347796701</v>
-      </c>
-      <c r="G14" s="29">
-        <v>0.22589851021766599</v>
-      </c>
-      <c r="H14" s="29">
-        <v>20</v>
-      </c>
-      <c r="I14" s="29"/>
-      <c r="J14" s="29" t="s">
-        <v>191</v>
-      </c>
-      <c r="K14" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A15" s="40"/>
-      <c r="B15" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="D15" s="29">
-        <v>0.33222808352364203</v>
-      </c>
-      <c r="E15" s="29">
-        <v>8.3754834143228804E-2</v>
-      </c>
-      <c r="F15" s="29">
-        <v>0.19432044552351499</v>
-      </c>
-      <c r="G15" s="32">
-        <v>0.234600452147424</v>
-      </c>
-      <c r="H15" s="29">
-        <v>20</v>
-      </c>
-      <c r="I15" s="29"/>
-      <c r="J15" s="29" t="s">
-        <v>192</v>
-      </c>
-      <c r="K15" s="29">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A16" s="40"/>
-      <c r="B16" s="29" t="s">
-        <v>168</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="D16" s="29">
-        <v>0.32203169576661</v>
-      </c>
-      <c r="E16" s="29">
-        <v>7.0582749966208697E-2</v>
-      </c>
-      <c r="F16" s="29">
-        <v>0.18391282196315101</v>
-      </c>
-      <c r="G16" s="29">
-        <v>0.20042349733412201</v>
-      </c>
-      <c r="H16" s="29">
-        <v>20</v>
-      </c>
-      <c r="I16" s="29"/>
-      <c r="J16" s="37" t="s">
-        <v>196</v>
-      </c>
-      <c r="K16" s="29">
-        <v>4</v>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" s="57" t="s">
+        <v>217</v>
+      </c>
+      <c r="B38" s="29">
+        <f>B36/F36</f>
+        <v>4.0411462160176341E-3</v>
+      </c>
+      <c r="C38" s="29">
+        <f>C36/G36</f>
+        <v>3.0983733539891559E-3</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="S1:S2"/>
-    <mergeCell ref="T1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="K1:K2"/>
+  <mergeCells count="21">
+    <mergeCell ref="O1:R1"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="H17:H21"/>
+    <mergeCell ref="H11:H16"/>
+    <mergeCell ref="H3:H6"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="A27:G27"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="A17:A21"/>
     <mergeCell ref="A11:A16"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="H1:H2"/>
-    <mergeCell ref="J1:J2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="A3:A6"/>
@@ -3703,42 +5444,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.35">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
-      <c r="F1" s="47" t="s">
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="47"/>
-      <c r="H1" s="47"/>
-      <c r="I1" s="47"/>
-      <c r="J1" s="47" t="s">
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="I1" s="44"/>
+      <c r="J1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="K1" s="47"/>
-      <c r="L1" s="47"/>
-      <c r="M1" s="47"/>
-      <c r="O1" s="47" t="s">
+      <c r="K1" s="44"/>
+      <c r="L1" s="44"/>
+      <c r="M1" s="44"/>
+      <c r="O1" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="P1" s="47"/>
-      <c r="Q1" s="47"/>
-      <c r="R1" s="47"/>
-      <c r="S1" s="47" t="s">
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+      <c r="S1" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="T1" s="47"/>
-      <c r="U1" s="47"/>
-      <c r="V1" s="47"/>
-      <c r="W1" s="47" t="s">
+      <c r="T1" s="44"/>
+      <c r="U1" s="44"/>
+      <c r="V1" s="44"/>
+      <c r="W1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="47"/>
-      <c r="Y1" s="47"/>
-      <c r="Z1" s="47"/>
+      <c r="X1" s="44"/>
+      <c r="Y1" s="44"/>
+      <c r="Z1" s="44"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
@@ -6635,21 +8376,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="F1" s="48" t="s">
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="F1" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="J1" s="48" t="s">
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="J1" s="45" t="s">
         <v>126</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
+      <c r="K1" s="45"/>
+      <c r="L1" s="45"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="14" t="s">

</xml_diff>